<commit_message>
ecran creation palanquees, fiche de sécurite, retrait limit 20 liste des adhérents
</commit_message>
<xml_diff>
--- a/APP_Fiche de securite_VLG.xlsx
+++ b/APP_Fiche de securite_VLG.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6780D2E2-9FA3-47D8-99E5-97A37EC03A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0571F7C8-3A80-4945-8F87-C5BEE6AF2E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28350" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12-05-2024" sheetId="7" r:id="rId1"/>
@@ -322,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +347,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="34">
     <border>
@@ -725,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -853,6 +859,147 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -868,149 +1015,35 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1109,7 +1142,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="50292" rIns="0" bIns="50292" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1195,7 +1228,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="50292" rIns="0" bIns="50292" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1232,7 +1265,7 @@
           <xdr:col>30</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>176213</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1281,7 +1314,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="50292" rIns="0" bIns="50292" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1310,7 +1343,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>30</xdr:col>
-          <xdr:colOff>214313</xdr:colOff>
+          <xdr:colOff>219075</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
@@ -1318,7 +1351,7 @@
           <xdr:col>34</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>176213</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1367,7 +1400,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="50292" rIns="0" bIns="50292" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1686,34 +1719,34 @@
   </sheetPr>
   <dimension ref="A1:AJ62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="AX28" sqref="AX28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="36"/>
-      <c r="D2" s="91">
+      <c r="D2" s="95">
         <v>45564</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
       <c r="K2" s="36"/>
@@ -1723,7 +1756,7 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="36" t="s">
+      <c r="P2" s="97" t="s">
         <v>42</v>
       </c>
       <c r="Q2" s="36"/>
@@ -1738,7 +1771,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="97" t="s">
         <v>43</v>
       </c>
       <c r="AB2" s="36"/>
@@ -1751,7 +1784,7 @@
       <c r="AI2" s="36"/>
       <c r="AJ2" s="5"/>
     </row>
-    <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
@@ -1783,12 +1816,12 @@
         <v>5</v>
       </c>
       <c r="Y3" s="7"/>
-      <c r="Z3" s="94" t="s">
+      <c r="Z3" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="95"/>
-      <c r="AB3" s="95"/>
-      <c r="AC3" s="95"/>
+      <c r="AA3" s="52"/>
+      <c r="AB3" s="52"/>
+      <c r="AC3" s="52"/>
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
@@ -1797,7 +1830,7 @@
       <c r="AI3" s="4"/>
       <c r="AJ3" s="5"/>
     </row>
-    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1841,7 +1874,7 @@
       <c r="AI4" s="9"/>
       <c r="AJ4" s="11"/>
     </row>
-    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1851,14 +1884,14 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="97"/>
       <c r="N5" s="36"/>
       <c r="O5" s="36"/>
       <c r="P5" s="36"/>
@@ -1883,83 +1916,83 @@
       <c r="AI5" s="4"/>
       <c r="AJ5" s="5"/>
     </row>
-    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="92" t="s">
+    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
-      <c r="P6" s="92"/>
-      <c r="Q6" s="92"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="92"/>
-      <c r="T6" s="92"/>
-      <c r="U6" s="92"/>
-      <c r="V6" s="92"/>
-      <c r="W6" s="92"/>
-      <c r="X6" s="92"/>
-      <c r="Y6" s="92"/>
-      <c r="Z6" s="92"/>
-      <c r="AA6" s="92"/>
-      <c r="AB6" s="92"/>
-      <c r="AC6" s="92"/>
-      <c r="AD6" s="92"/>
-      <c r="AE6" s="92"/>
-      <c r="AF6" s="92"/>
-      <c r="AG6" s="92"/>
-      <c r="AH6" s="92"/>
-    </row>
-    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="93" t="s">
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="44"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="44"/>
+      <c r="X6" s="44"/>
+      <c r="Y6" s="44"/>
+      <c r="Z6" s="44"/>
+      <c r="AA6" s="44"/>
+      <c r="AB6" s="44"/>
+      <c r="AC6" s="44"/>
+      <c r="AD6" s="44"/>
+      <c r="AE6" s="44"/>
+      <c r="AF6" s="44"/>
+      <c r="AG6" s="44"/>
+      <c r="AH6" s="44"/>
+    </row>
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="93"/>
-      <c r="N7" s="93"/>
-      <c r="O7" s="93"/>
-      <c r="P7" s="93"/>
-      <c r="Q7" s="93"/>
-      <c r="R7" s="93"/>
-      <c r="S7" s="93"/>
-      <c r="T7" s="93"/>
-      <c r="U7" s="93"/>
-      <c r="V7" s="93"/>
-      <c r="W7" s="93"/>
-      <c r="X7" s="93"/>
-      <c r="Y7" s="93"/>
-      <c r="Z7" s="93"/>
-      <c r="AA7" s="93"/>
-      <c r="AB7" s="93"/>
-      <c r="AC7" s="93"/>
-      <c r="AD7" s="93"/>
-      <c r="AE7" s="93"/>
-      <c r="AF7" s="93"/>
-      <c r="AG7" s="93"/>
-      <c r="AH7" s="93"/>
-    </row>
-    <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="45"/>
+      <c r="AA7" s="45"/>
+      <c r="AB7" s="45"/>
+      <c r="AC7" s="45"/>
+      <c r="AD7" s="45"/>
+      <c r="AE7" s="45"/>
+      <c r="AF7" s="45"/>
+      <c r="AG7" s="45"/>
+      <c r="AH7" s="45"/>
+    </row>
+    <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>13</v>
       </c>
@@ -2003,7 +2036,7 @@
       <c r="AI8" s="19"/>
       <c r="AJ8" s="22"/>
     </row>
-    <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
@@ -2047,7 +2080,7 @@
       <c r="AI9" s="4"/>
       <c r="AJ9" s="5"/>
     </row>
-    <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="40"/>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -2085,7 +2118,7 @@
       <c r="AI10" s="4"/>
       <c r="AJ10" s="5"/>
     </row>
-    <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -2123,7 +2156,7 @@
       <c r="AI11" s="4"/>
       <c r="AJ11" s="5"/>
     </row>
-    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -2161,7 +2194,7 @@
       <c r="AI12" s="4"/>
       <c r="AJ12" s="5"/>
     </row>
-    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
@@ -2199,7 +2232,7 @@
       <c r="AI13" s="4"/>
       <c r="AJ13" s="5"/>
     </row>
-    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
@@ -2237,247 +2270,247 @@
       <c r="AI14" s="4"/>
       <c r="AJ14" s="5"/>
     </row>
-    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="93" t="s">
+    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="93"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="93"/>
-      <c r="L16" s="93"/>
-      <c r="M16" s="93"/>
-      <c r="N16" s="93"/>
-      <c r="O16" s="93"/>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93"/>
-      <c r="S16" s="93"/>
-      <c r="T16" s="93"/>
-      <c r="U16" s="93"/>
-      <c r="V16" s="93"/>
-      <c r="W16" s="93"/>
-      <c r="X16" s="93"/>
-      <c r="Y16" s="93"/>
-      <c r="Z16" s="93"/>
-      <c r="AA16" s="93"/>
-      <c r="AB16" s="93"/>
-      <c r="AC16" s="93"/>
-      <c r="AD16" s="93"/>
-      <c r="AE16" s="93"/>
-      <c r="AF16" s="93"/>
-      <c r="AG16" s="93"/>
-      <c r="AH16" s="93"/>
-      <c r="AI16" s="93"/>
-      <c r="AJ16" s="93"/>
-    </row>
-    <row r="17" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="75" t="s">
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="45"/>
+      <c r="X16" s="45"/>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="45"/>
+      <c r="AA16" s="45"/>
+      <c r="AB16" s="45"/>
+      <c r="AC16" s="45"/>
+      <c r="AD16" s="45"/>
+      <c r="AE16" s="45"/>
+      <c r="AF16" s="45"/>
+      <c r="AG16" s="45"/>
+      <c r="AH16" s="45"/>
+      <c r="AI16" s="45"/>
+      <c r="AJ16" s="45"/>
+    </row>
+    <row r="17" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="75" t="s">
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="76"/>
-      <c r="L17" s="78"/>
-      <c r="M17" s="79" t="s">
+      <c r="K17" s="47"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="77"/>
-      <c r="V17" s="75" t="s">
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="W17" s="76"/>
-      <c r="X17" s="78"/>
-      <c r="Y17" s="79" t="s">
+      <c r="W17" s="47"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="Z17" s="76"/>
-      <c r="AA17" s="76"/>
-      <c r="AB17" s="76"/>
-      <c r="AC17" s="76"/>
-      <c r="AD17" s="76"/>
-      <c r="AE17" s="76"/>
-      <c r="AF17" s="76"/>
-      <c r="AG17" s="77"/>
-      <c r="AH17" s="75" t="s">
+      <c r="Z17" s="47"/>
+      <c r="AA17" s="47"/>
+      <c r="AB17" s="47"/>
+      <c r="AC17" s="47"/>
+      <c r="AD17" s="47"/>
+      <c r="AE17" s="47"/>
+      <c r="AF17" s="47"/>
+      <c r="AG17" s="48"/>
+      <c r="AH17" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="AI17" s="76"/>
-      <c r="AJ17" s="77"/>
-    </row>
-    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="40" t="s">
+      <c r="AI17" s="47"/>
+      <c r="AJ17" s="48"/>
+    </row>
+    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="71" t="s">
+      <c r="B18" s="97"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="99"/>
+      <c r="J18" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="72"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="38" t="s">
+      <c r="K18" s="96"/>
+      <c r="L18" s="101"/>
+      <c r="M18" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
+      <c r="N18" s="97"/>
+      <c r="O18" s="97"/>
+      <c r="P18" s="97"/>
+      <c r="Q18" s="97"/>
+      <c r="R18" s="97"/>
+      <c r="S18" s="97"/>
+      <c r="T18" s="97"/>
       <c r="U18" s="39"/>
-      <c r="V18" s="71" t="s">
+      <c r="V18" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="W18" s="72"/>
-      <c r="X18" s="73"/>
-      <c r="Y18" s="38" t="s">
+      <c r="W18" s="96"/>
+      <c r="X18" s="101"/>
+      <c r="Y18" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="Z18" s="36"/>
-      <c r="AA18" s="36"/>
-      <c r="AB18" s="36"/>
-      <c r="AC18" s="36"/>
-      <c r="AD18" s="36"/>
-      <c r="AE18" s="36"/>
-      <c r="AF18" s="36"/>
-      <c r="AG18" s="39"/>
-      <c r="AH18" s="71" t="s">
+      <c r="Z18" s="97"/>
+      <c r="AA18" s="97"/>
+      <c r="AB18" s="97"/>
+      <c r="AC18" s="97"/>
+      <c r="AD18" s="97"/>
+      <c r="AE18" s="97"/>
+      <c r="AF18" s="97"/>
+      <c r="AG18" s="99"/>
+      <c r="AH18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="AI18" s="72"/>
-      <c r="AJ18" s="74"/>
-    </row>
-    <row r="19" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="75" t="s">
+      <c r="AI18" s="96"/>
+      <c r="AJ18" s="104"/>
+    </row>
+    <row r="19" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="77"/>
-      <c r="J19" s="75" t="s">
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="76"/>
-      <c r="L19" s="78"/>
-      <c r="M19" s="79" t="s">
+      <c r="K19" s="47"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="N19" s="76"/>
-      <c r="O19" s="76"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="76"/>
-      <c r="S19" s="76"/>
-      <c r="T19" s="76"/>
-      <c r="U19" s="77"/>
-      <c r="V19" s="75" t="s">
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="47"/>
+      <c r="S19" s="47"/>
+      <c r="T19" s="47"/>
+      <c r="U19" s="48"/>
+      <c r="V19" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="W19" s="76"/>
-      <c r="X19" s="78"/>
-      <c r="Y19" s="79" t="s">
+      <c r="W19" s="47"/>
+      <c r="X19" s="49"/>
+      <c r="Y19" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="Z19" s="76"/>
-      <c r="AA19" s="76"/>
-      <c r="AB19" s="76"/>
-      <c r="AC19" s="76"/>
-      <c r="AD19" s="76"/>
-      <c r="AE19" s="76"/>
-      <c r="AF19" s="76"/>
-      <c r="AG19" s="77"/>
-      <c r="AH19" s="75" t="s">
+      <c r="Z19" s="47"/>
+      <c r="AA19" s="47"/>
+      <c r="AB19" s="47"/>
+      <c r="AC19" s="47"/>
+      <c r="AD19" s="47"/>
+      <c r="AE19" s="47"/>
+      <c r="AF19" s="47"/>
+      <c r="AG19" s="48"/>
+      <c r="AH19" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="AI19" s="76"/>
-      <c r="AJ19" s="77"/>
-    </row>
-    <row r="20" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="40" t="s">
+      <c r="AI19" s="47"/>
+      <c r="AJ19" s="48"/>
+    </row>
+    <row r="20" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="71" t="s">
+      <c r="B20" s="97"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="99"/>
+      <c r="J20" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="K20" s="72"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="38" t="s">
+      <c r="K20" s="96"/>
+      <c r="L20" s="101"/>
+      <c r="M20" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="39"/>
-      <c r="V20" s="71" t="s">
+      <c r="N20" s="97"/>
+      <c r="O20" s="97"/>
+      <c r="P20" s="97"/>
+      <c r="Q20" s="97"/>
+      <c r="R20" s="97"/>
+      <c r="S20" s="97"/>
+      <c r="T20" s="97"/>
+      <c r="U20" s="99"/>
+      <c r="V20" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="W20" s="72"/>
-      <c r="X20" s="73"/>
-      <c r="Y20" s="40" t="s">
+      <c r="W20" s="96"/>
+      <c r="X20" s="101"/>
+      <c r="Y20" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="Z20" s="36"/>
-      <c r="AA20" s="36"/>
-      <c r="AB20" s="36"/>
-      <c r="AC20" s="36"/>
-      <c r="AD20" s="36"/>
-      <c r="AE20" s="36"/>
+      <c r="Z20" s="97"/>
+      <c r="AA20" s="97"/>
+      <c r="AB20" s="97"/>
+      <c r="AC20" s="97"/>
+      <c r="AD20" s="97"/>
+      <c r="AE20" s="97"/>
       <c r="AF20" s="36"/>
       <c r="AG20" s="39"/>
-      <c r="AH20" s="71" t="s">
+      <c r="AH20" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="AI20" s="72"/>
-      <c r="AJ20" s="74"/>
-    </row>
-    <row r="21" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AI20" s="96"/>
+      <c r="AJ20" s="104"/>
+    </row>
+    <row r="21" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -2487,9 +2520,9 @@
       <c r="G21" s="36"/>
       <c r="H21" s="36"/>
       <c r="I21" s="39"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="73"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="54"/>
       <c r="M21" s="38"/>
       <c r="N21" s="36"/>
       <c r="O21" s="36"/>
@@ -2499,9 +2532,9 @@
       <c r="S21" s="36"/>
       <c r="T21" s="36"/>
       <c r="U21" s="39"/>
-      <c r="V21" s="71"/>
-      <c r="W21" s="72"/>
-      <c r="X21" s="73"/>
+      <c r="V21" s="53"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="54"/>
       <c r="Y21" s="38"/>
       <c r="Z21" s="36"/>
       <c r="AA21" s="36"/>
@@ -2511,11 +2544,11 @@
       <c r="AE21" s="36"/>
       <c r="AF21" s="36"/>
       <c r="AG21" s="39"/>
-      <c r="AH21" s="71"/>
-      <c r="AI21" s="72"/>
-      <c r="AJ21" s="74"/>
-    </row>
-    <row r="22" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH21" s="53"/>
+      <c r="AI21" s="43"/>
+      <c r="AJ21" s="55"/>
+    </row>
+    <row r="22" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -2525,9 +2558,9 @@
       <c r="G22" s="36"/>
       <c r="H22" s="36"/>
       <c r="I22" s="39"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="73"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="54"/>
       <c r="M22" s="38"/>
       <c r="N22" s="36"/>
       <c r="O22" s="36"/>
@@ -2537,9 +2570,9 @@
       <c r="S22" s="36"/>
       <c r="T22" s="36"/>
       <c r="U22" s="39"/>
-      <c r="V22" s="71"/>
-      <c r="W22" s="72"/>
-      <c r="X22" s="73"/>
+      <c r="V22" s="53"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="54"/>
       <c r="Y22" s="38"/>
       <c r="Z22" s="36"/>
       <c r="AA22" s="36"/>
@@ -2549,11 +2582,11 @@
       <c r="AE22" s="36"/>
       <c r="AF22" s="36"/>
       <c r="AG22" s="39"/>
-      <c r="AH22" s="71"/>
-      <c r="AI22" s="72"/>
-      <c r="AJ22" s="74"/>
-    </row>
-    <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH22" s="53"/>
+      <c r="AI22" s="43"/>
+      <c r="AJ22" s="55"/>
+    </row>
+    <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
@@ -2563,9 +2596,9 @@
       <c r="G23" s="36"/>
       <c r="H23" s="36"/>
       <c r="I23" s="39"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="73"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="54"/>
       <c r="M23" s="38"/>
       <c r="N23" s="36"/>
       <c r="O23" s="36"/>
@@ -2575,9 +2608,9 @@
       <c r="S23" s="36"/>
       <c r="T23" s="36"/>
       <c r="U23" s="39"/>
-      <c r="V23" s="71"/>
-      <c r="W23" s="72"/>
-      <c r="X23" s="73"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="54"/>
       <c r="Y23" s="38"/>
       <c r="Z23" s="36"/>
       <c r="AA23" s="36"/>
@@ -2587,279 +2620,279 @@
       <c r="AE23" s="36"/>
       <c r="AF23" s="36"/>
       <c r="AG23" s="39"/>
-      <c r="AH23" s="71"/>
-      <c r="AI23" s="72"/>
-      <c r="AJ23" s="74"/>
-    </row>
-    <row r="24" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="61" t="s">
+      <c r="AH23" s="53"/>
+      <c r="AI23" s="43"/>
+      <c r="AJ23" s="55"/>
+    </row>
+    <row r="24" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="63"/>
-      <c r="M24" s="64" t="s">
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="N24" s="62"/>
-      <c r="O24" s="62"/>
-      <c r="P24" s="62"/>
-      <c r="Q24" s="62"/>
-      <c r="R24" s="62"/>
-      <c r="S24" s="62"/>
-      <c r="T24" s="62"/>
-      <c r="U24" s="62"/>
-      <c r="V24" s="62"/>
-      <c r="W24" s="62"/>
-      <c r="X24" s="63"/>
-      <c r="Y24" s="64" t="s">
+      <c r="N24" s="57"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="57"/>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="57"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="58"/>
+      <c r="Y24" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="Z24" s="62"/>
-      <c r="AA24" s="62"/>
-      <c r="AB24" s="62"/>
-      <c r="AC24" s="62"/>
-      <c r="AD24" s="62"/>
-      <c r="AE24" s="62"/>
-      <c r="AF24" s="62"/>
-      <c r="AG24" s="62"/>
-      <c r="AH24" s="62"/>
-      <c r="AI24" s="62"/>
-      <c r="AJ24" s="65"/>
-    </row>
-    <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="66" t="s">
+      <c r="Z24" s="57"/>
+      <c r="AA24" s="57"/>
+      <c r="AB24" s="57"/>
+      <c r="AC24" s="57"/>
+      <c r="AD24" s="57"/>
+      <c r="AE24" s="57"/>
+      <c r="AF24" s="57"/>
+      <c r="AG24" s="57"/>
+      <c r="AH24" s="57"/>
+      <c r="AI24" s="57"/>
+      <c r="AJ24" s="60"/>
+    </row>
+    <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="41">
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="103">
         <v>6</v>
       </c>
       <c r="G25" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="67" t="s">
+      <c r="H25" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="67"/>
-      <c r="J25" s="41">
+      <c r="I25" s="62"/>
+      <c r="J25" s="103">
         <v>40</v>
       </c>
-      <c r="K25" s="68" t="s">
+      <c r="K25" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="L25" s="69"/>
-      <c r="M25" s="66" t="s">
+      <c r="L25" s="64"/>
+      <c r="M25" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="67"/>
-      <c r="O25" s="67"/>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="67"/>
-      <c r="R25" s="41">
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
+      <c r="R25" s="103">
         <v>6</v>
       </c>
       <c r="S25" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="T25" s="67" t="s">
+      <c r="T25" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="U25" s="67"/>
-      <c r="V25" s="41">
+      <c r="U25" s="62"/>
+      <c r="V25" s="103">
         <v>40</v>
       </c>
-      <c r="W25" s="68" t="s">
+      <c r="W25" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="X25" s="69"/>
-      <c r="Y25" s="66" t="s">
+      <c r="X25" s="64"/>
+      <c r="Y25" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Z25" s="67"/>
-      <c r="AA25" s="67"/>
-      <c r="AB25" s="67"/>
-      <c r="AC25" s="67"/>
+      <c r="Z25" s="62"/>
+      <c r="AA25" s="62"/>
+      <c r="AB25" s="62"/>
+      <c r="AC25" s="62"/>
       <c r="AD25" s="41">
         <v>6</v>
       </c>
       <c r="AE25" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="AF25" s="67" t="s">
+      <c r="AF25" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="AG25" s="67"/>
+      <c r="AG25" s="62"/>
       <c r="AH25" s="41">
         <v>40</v>
       </c>
-      <c r="AI25" s="68" t="s">
+      <c r="AI25" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AJ25" s="70"/>
-    </row>
-    <row r="26" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="48" t="s">
+      <c r="AJ25" s="68"/>
+    </row>
+    <row r="26" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="51" t="s">
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="49"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="49"/>
-      <c r="S26" s="49"/>
-      <c r="T26" s="49"/>
-      <c r="U26" s="49"/>
-      <c r="V26" s="49"/>
-      <c r="W26" s="49"/>
-      <c r="X26" s="50"/>
-      <c r="Y26" s="51" t="s">
+      <c r="N26" s="70"/>
+      <c r="O26" s="70"/>
+      <c r="P26" s="70"/>
+      <c r="Q26" s="70"/>
+      <c r="R26" s="70"/>
+      <c r="S26" s="70"/>
+      <c r="T26" s="70"/>
+      <c r="U26" s="70"/>
+      <c r="V26" s="70"/>
+      <c r="W26" s="70"/>
+      <c r="X26" s="71"/>
+      <c r="Y26" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="Z26" s="49"/>
-      <c r="AA26" s="49"/>
-      <c r="AB26" s="49"/>
-      <c r="AC26" s="49"/>
-      <c r="AD26" s="49"/>
-      <c r="AE26" s="49"/>
-      <c r="AF26" s="49"/>
-      <c r="AG26" s="49"/>
-      <c r="AH26" s="49"/>
-      <c r="AI26" s="49"/>
-      <c r="AJ26" s="52"/>
-    </row>
-    <row r="27" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="53" t="s">
+      <c r="Z26" s="70"/>
+      <c r="AA26" s="70"/>
+      <c r="AB26" s="70"/>
+      <c r="AC26" s="70"/>
+      <c r="AD26" s="70"/>
+      <c r="AE26" s="70"/>
+      <c r="AF26" s="70"/>
+      <c r="AG26" s="70"/>
+      <c r="AH26" s="70"/>
+      <c r="AI26" s="70"/>
+      <c r="AJ26" s="73"/>
+    </row>
+    <row r="27" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54" t="s">
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="56" t="s">
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="N27" s="54"/>
-      <c r="O27" s="54"/>
-      <c r="P27" s="54"/>
-      <c r="Q27" s="54"/>
-      <c r="R27" s="54"/>
-      <c r="S27" s="54"/>
-      <c r="T27" s="54"/>
-      <c r="U27" s="54" t="s">
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="65"/>
+      <c r="T27" s="65"/>
+      <c r="U27" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="V27" s="54"/>
-      <c r="W27" s="54"/>
-      <c r="X27" s="55"/>
-      <c r="Y27" s="56" t="s">
+      <c r="V27" s="65"/>
+      <c r="W27" s="65"/>
+      <c r="X27" s="67"/>
+      <c r="Y27" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="Z27" s="54"/>
-      <c r="AA27" s="54"/>
-      <c r="AB27" s="54"/>
-      <c r="AC27" s="54"/>
-      <c r="AD27" s="54"/>
-      <c r="AE27" s="54"/>
-      <c r="AF27" s="54"/>
-      <c r="AG27" s="54" t="s">
+      <c r="Z27" s="65"/>
+      <c r="AA27" s="65"/>
+      <c r="AB27" s="65"/>
+      <c r="AC27" s="65"/>
+      <c r="AD27" s="65"/>
+      <c r="AE27" s="65"/>
+      <c r="AF27" s="65"/>
+      <c r="AG27" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="AH27" s="54"/>
-      <c r="AI27" s="54"/>
-      <c r="AJ27" s="57"/>
-    </row>
-    <row r="28" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH27" s="65"/>
+      <c r="AI27" s="65"/>
+      <c r="AJ27" s="66"/>
+    </row>
+    <row r="28" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
       <c r="D28" s="23"/>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54" t="s">
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="54"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="55"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="67"/>
       <c r="M28" s="24" t="s">
         <v>22</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
       <c r="P28" s="23"/>
-      <c r="Q28" s="54" t="s">
+      <c r="Q28" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="R28" s="54"/>
-      <c r="S28" s="54"/>
-      <c r="T28" s="54"/>
-      <c r="U28" s="54" t="s">
+      <c r="R28" s="65"/>
+      <c r="S28" s="65"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="V28" s="54"/>
-      <c r="W28" s="54"/>
-      <c r="X28" s="55"/>
+      <c r="V28" s="65"/>
+      <c r="W28" s="65"/>
+      <c r="X28" s="67"/>
       <c r="Y28" s="24" t="s">
         <v>22</v>
       </c>
       <c r="Z28" s="23"/>
       <c r="AA28" s="23"/>
       <c r="AB28" s="23"/>
-      <c r="AC28" s="54" t="s">
+      <c r="AC28" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AD28" s="54"/>
-      <c r="AE28" s="54"/>
-      <c r="AF28" s="54"/>
-      <c r="AG28" s="54" t="s">
+      <c r="AD28" s="65"/>
+      <c r="AE28" s="65"/>
+      <c r="AF28" s="65"/>
+      <c r="AG28" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="AH28" s="54"/>
-      <c r="AI28" s="54"/>
-      <c r="AJ28" s="57"/>
-    </row>
-    <row r="29" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AH28" s="65"/>
+      <c r="AI28" s="65"/>
+      <c r="AJ28" s="66"/>
+    </row>
+    <row r="29" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="28"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
@@ -2909,39 +2942,39 @@
       <c r="AI29" s="84"/>
       <c r="AJ29" s="86"/>
     </row>
-    <row r="30" spans="1:36" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="87" t="s">
+    <row r="30" spans="1:36" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="88"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="88"/>
-      <c r="H30" s="88"/>
-      <c r="I30" s="89"/>
-      <c r="J30" s="87" t="s">
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="78"/>
+      <c r="J30" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="K30" s="88"/>
-      <c r="L30" s="90"/>
-      <c r="M30" s="87" t="s">
+      <c r="K30" s="77"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="N30" s="88"/>
-      <c r="O30" s="88"/>
-      <c r="P30" s="88"/>
-      <c r="Q30" s="88"/>
-      <c r="R30" s="88"/>
-      <c r="S30" s="88"/>
-      <c r="T30" s="88"/>
-      <c r="U30" s="89"/>
-      <c r="V30" s="87" t="s">
+      <c r="N30" s="77"/>
+      <c r="O30" s="77"/>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="77"/>
+      <c r="R30" s="77"/>
+      <c r="S30" s="77"/>
+      <c r="T30" s="77"/>
+      <c r="U30" s="78"/>
+      <c r="V30" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="W30" s="88"/>
-      <c r="X30" s="90"/>
+      <c r="W30" s="77"/>
+      <c r="X30" s="79"/>
       <c r="Y30" s="80" t="s">
         <v>16</v>
       </c>
@@ -2959,7 +2992,7 @@
       <c r="AI30" s="81"/>
       <c r="AJ30" s="82"/>
     </row>
-    <row r="31" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>55</v>
       </c>
@@ -2971,11 +3004,11 @@
       <c r="G31" s="36"/>
       <c r="H31" s="36"/>
       <c r="I31" s="39"/>
-      <c r="J31" s="71" t="s">
+      <c r="J31" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="K31" s="72"/>
-      <c r="L31" s="73"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="54"/>
       <c r="M31" s="40" t="s">
         <v>62</v>
       </c>
@@ -2987,11 +3020,11 @@
       <c r="S31" s="36"/>
       <c r="T31" s="36"/>
       <c r="U31" s="39"/>
-      <c r="V31" s="71" t="s">
+      <c r="V31" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="W31" s="72"/>
-      <c r="X31" s="73"/>
+      <c r="W31" s="43"/>
+      <c r="X31" s="54"/>
       <c r="Y31" s="38" t="s">
         <v>49</v>
       </c>
@@ -3003,63 +3036,63 @@
       <c r="AE31" s="36"/>
       <c r="AF31" s="36"/>
       <c r="AG31" s="39"/>
-      <c r="AH31" s="71" t="s">
+      <c r="AH31" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="AI31" s="72"/>
-      <c r="AJ31" s="74"/>
-    </row>
-    <row r="32" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="75" t="s">
+      <c r="AI31" s="43"/>
+      <c r="AJ31" s="55"/>
+    </row>
+    <row r="32" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="76"/>
-      <c r="H32" s="76"/>
-      <c r="I32" s="77"/>
-      <c r="J32" s="75" t="s">
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="76"/>
-      <c r="L32" s="78"/>
-      <c r="M32" s="75" t="s">
+      <c r="K32" s="47"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="N32" s="76"/>
-      <c r="O32" s="76"/>
-      <c r="P32" s="76"/>
-      <c r="Q32" s="76"/>
-      <c r="R32" s="76"/>
-      <c r="S32" s="76"/>
-      <c r="T32" s="76"/>
-      <c r="U32" s="77"/>
-      <c r="V32" s="75" t="s">
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="47"/>
+      <c r="Q32" s="47"/>
+      <c r="R32" s="47"/>
+      <c r="S32" s="47"/>
+      <c r="T32" s="47"/>
+      <c r="U32" s="48"/>
+      <c r="V32" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="W32" s="76"/>
-      <c r="X32" s="78"/>
-      <c r="Y32" s="79" t="s">
+      <c r="W32" s="47"/>
+      <c r="X32" s="49"/>
+      <c r="Y32" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="Z32" s="76"/>
-      <c r="AA32" s="76"/>
-      <c r="AB32" s="76"/>
-      <c r="AC32" s="76"/>
-      <c r="AD32" s="76"/>
-      <c r="AE32" s="76"/>
-      <c r="AF32" s="76"/>
-      <c r="AG32" s="77"/>
-      <c r="AH32" s="75" t="s">
+      <c r="Z32" s="47"/>
+      <c r="AA32" s="47"/>
+      <c r="AB32" s="47"/>
+      <c r="AC32" s="47"/>
+      <c r="AD32" s="47"/>
+      <c r="AE32" s="47"/>
+      <c r="AF32" s="47"/>
+      <c r="AG32" s="48"/>
+      <c r="AH32" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="AI32" s="76"/>
-      <c r="AJ32" s="77"/>
-    </row>
-    <row r="33" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AI32" s="47"/>
+      <c r="AJ32" s="48"/>
+    </row>
+    <row r="33" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
         <v>56</v>
       </c>
@@ -3071,11 +3104,11 @@
       <c r="G33" s="36"/>
       <c r="H33" s="36"/>
       <c r="I33" s="39"/>
-      <c r="J33" s="71" t="s">
+      <c r="J33" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="K33" s="72"/>
-      <c r="L33" s="73"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="54"/>
       <c r="M33" s="40" t="s">
         <v>57</v>
       </c>
@@ -3087,11 +3120,11 @@
       <c r="S33" s="36"/>
       <c r="T33" s="36"/>
       <c r="U33" s="39"/>
-      <c r="V33" s="71" t="s">
+      <c r="V33" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="W33" s="72"/>
-      <c r="X33" s="73"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="54"/>
       <c r="Y33" s="38" t="s">
         <v>58</v>
       </c>
@@ -3103,13 +3136,13 @@
       <c r="AE33" s="36"/>
       <c r="AF33" s="36"/>
       <c r="AG33" s="39"/>
-      <c r="AH33" s="71" t="s">
+      <c r="AH33" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="AI33" s="72"/>
-      <c r="AJ33" s="74"/>
-    </row>
-    <row r="34" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AI33" s="43"/>
+      <c r="AJ33" s="55"/>
+    </row>
+    <row r="34" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="36"/>
       <c r="C34" s="36"/>
@@ -3119,9 +3152,9 @@
       <c r="G34" s="36"/>
       <c r="H34" s="36"/>
       <c r="I34" s="39"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="72"/>
-      <c r="L34" s="73"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="54"/>
       <c r="M34" s="40"/>
       <c r="N34" s="36"/>
       <c r="O34" s="36"/>
@@ -3131,9 +3164,9 @@
       <c r="S34" s="36"/>
       <c r="T34" s="36"/>
       <c r="U34" s="39"/>
-      <c r="V34" s="71"/>
-      <c r="W34" s="72"/>
-      <c r="X34" s="73"/>
+      <c r="V34" s="53"/>
+      <c r="W34" s="43"/>
+      <c r="X34" s="54"/>
       <c r="Y34" s="38"/>
       <c r="Z34" s="36"/>
       <c r="AA34" s="36"/>
@@ -3143,11 +3176,11 @@
       <c r="AE34" s="36"/>
       <c r="AF34" s="36"/>
       <c r="AG34" s="39"/>
-      <c r="AH34" s="71"/>
-      <c r="AI34" s="72"/>
-      <c r="AJ34" s="74"/>
-    </row>
-    <row r="35" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH34" s="53"/>
+      <c r="AI34" s="43"/>
+      <c r="AJ34" s="55"/>
+    </row>
+    <row r="35" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="36"/>
       <c r="C35" s="36"/>
@@ -3157,9 +3190,9 @@
       <c r="G35" s="36"/>
       <c r="H35" s="36"/>
       <c r="I35" s="39"/>
-      <c r="J35" s="71"/>
-      <c r="K35" s="72"/>
-      <c r="L35" s="73"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="54"/>
       <c r="M35" s="40"/>
       <c r="N35" s="36"/>
       <c r="O35" s="36"/>
@@ -3169,9 +3202,9 @@
       <c r="S35" s="36"/>
       <c r="T35" s="36"/>
       <c r="U35" s="39"/>
-      <c r="V35" s="71"/>
-      <c r="W35" s="72"/>
-      <c r="X35" s="73"/>
+      <c r="V35" s="53"/>
+      <c r="W35" s="43"/>
+      <c r="X35" s="54"/>
       <c r="Y35" s="38"/>
       <c r="Z35" s="36"/>
       <c r="AA35" s="36"/>
@@ -3181,11 +3214,11 @@
       <c r="AE35" s="36"/>
       <c r="AF35" s="36"/>
       <c r="AG35" s="39"/>
-      <c r="AH35" s="71"/>
-      <c r="AI35" s="72"/>
-      <c r="AJ35" s="74"/>
-    </row>
-    <row r="36" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH35" s="53"/>
+      <c r="AI35" s="43"/>
+      <c r="AJ35" s="55"/>
+    </row>
+    <row r="36" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
       <c r="B36" s="36"/>
       <c r="C36" s="36"/>
@@ -3195,9 +3228,9 @@
       <c r="G36" s="36"/>
       <c r="H36" s="36"/>
       <c r="I36" s="39"/>
-      <c r="J36" s="71"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="73"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="54"/>
       <c r="M36" s="40"/>
       <c r="N36" s="36"/>
       <c r="O36" s="36"/>
@@ -3207,9 +3240,9 @@
       <c r="S36" s="36"/>
       <c r="T36" s="36"/>
       <c r="U36" s="39"/>
-      <c r="V36" s="71"/>
-      <c r="W36" s="72"/>
-      <c r="X36" s="73"/>
+      <c r="V36" s="53"/>
+      <c r="W36" s="43"/>
+      <c r="X36" s="54"/>
       <c r="Y36" s="38"/>
       <c r="Z36" s="36"/>
       <c r="AA36" s="36"/>
@@ -3219,279 +3252,279 @@
       <c r="AE36" s="36"/>
       <c r="AF36" s="36"/>
       <c r="AG36" s="39"/>
-      <c r="AH36" s="71"/>
-      <c r="AI36" s="72"/>
-      <c r="AJ36" s="74"/>
-    </row>
-    <row r="37" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="61" t="s">
+      <c r="AH36" s="53"/>
+      <c r="AI36" s="43"/>
+      <c r="AJ36" s="55"/>
+    </row>
+    <row r="37" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="62"/>
-      <c r="K37" s="62"/>
-      <c r="L37" s="63"/>
-      <c r="M37" s="64" t="s">
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="N37" s="62"/>
-      <c r="O37" s="62"/>
-      <c r="P37" s="62"/>
-      <c r="Q37" s="62"/>
-      <c r="R37" s="62"/>
-      <c r="S37" s="62"/>
-      <c r="T37" s="62"/>
-      <c r="U37" s="62"/>
-      <c r="V37" s="62"/>
-      <c r="W37" s="62"/>
-      <c r="X37" s="65"/>
-      <c r="Y37" s="64" t="s">
+      <c r="N37" s="57"/>
+      <c r="O37" s="57"/>
+      <c r="P37" s="57"/>
+      <c r="Q37" s="57"/>
+      <c r="R37" s="57"/>
+      <c r="S37" s="57"/>
+      <c r="T37" s="57"/>
+      <c r="U37" s="57"/>
+      <c r="V37" s="57"/>
+      <c r="W37" s="57"/>
+      <c r="X37" s="60"/>
+      <c r="Y37" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="Z37" s="62"/>
-      <c r="AA37" s="62"/>
-      <c r="AB37" s="62"/>
-      <c r="AC37" s="62"/>
-      <c r="AD37" s="62"/>
-      <c r="AE37" s="62"/>
-      <c r="AF37" s="62"/>
-      <c r="AG37" s="62"/>
-      <c r="AH37" s="62"/>
-      <c r="AI37" s="62"/>
-      <c r="AJ37" s="65"/>
-    </row>
-    <row r="38" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="66" t="s">
+      <c r="Z37" s="57"/>
+      <c r="AA37" s="57"/>
+      <c r="AB37" s="57"/>
+      <c r="AC37" s="57"/>
+      <c r="AD37" s="57"/>
+      <c r="AE37" s="57"/>
+      <c r="AF37" s="57"/>
+      <c r="AG37" s="57"/>
+      <c r="AH37" s="57"/>
+      <c r="AI37" s="57"/>
+      <c r="AJ37" s="60"/>
+    </row>
+    <row r="38" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="67"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="67"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="41">
         <v>6</v>
       </c>
       <c r="G38" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="67" t="s">
+      <c r="H38" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="I38" s="67"/>
+      <c r="I38" s="62"/>
       <c r="J38" s="41">
         <v>40</v>
       </c>
-      <c r="K38" s="68" t="s">
+      <c r="K38" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="L38" s="69"/>
-      <c r="M38" s="66" t="s">
+      <c r="L38" s="64"/>
+      <c r="M38" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="N38" s="67"/>
-      <c r="O38" s="67"/>
-      <c r="P38" s="67"/>
-      <c r="Q38" s="67"/>
+      <c r="N38" s="62"/>
+      <c r="O38" s="62"/>
+      <c r="P38" s="62"/>
+      <c r="Q38" s="62"/>
       <c r="R38" s="41">
         <v>6</v>
       </c>
       <c r="S38" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="T38" s="67" t="s">
+      <c r="T38" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="U38" s="67"/>
+      <c r="U38" s="62"/>
       <c r="V38" s="41">
         <v>40</v>
       </c>
-      <c r="W38" s="68" t="s">
+      <c r="W38" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="X38" s="69"/>
-      <c r="Y38" s="66" t="s">
+      <c r="X38" s="64"/>
+      <c r="Y38" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Z38" s="67"/>
-      <c r="AA38" s="67"/>
-      <c r="AB38" s="67"/>
-      <c r="AC38" s="67"/>
+      <c r="Z38" s="62"/>
+      <c r="AA38" s="62"/>
+      <c r="AB38" s="62"/>
+      <c r="AC38" s="62"/>
       <c r="AD38" s="41">
         <v>6</v>
       </c>
       <c r="AE38" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="AF38" s="67" t="s">
+      <c r="AF38" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="AG38" s="67"/>
+      <c r="AG38" s="62"/>
       <c r="AH38" s="41">
         <v>40</v>
       </c>
-      <c r="AI38" s="68" t="s">
+      <c r="AI38" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AJ38" s="70"/>
-    </row>
-    <row r="39" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="48" t="s">
+      <c r="AJ38" s="68"/>
+    </row>
+    <row r="39" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="51" t="s">
+      <c r="B39" s="70"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70"/>
+      <c r="L39" s="71"/>
+      <c r="M39" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="49"/>
-      <c r="S39" s="49"/>
-      <c r="T39" s="49"/>
-      <c r="U39" s="49"/>
-      <c r="V39" s="49"/>
-      <c r="W39" s="49"/>
-      <c r="X39" s="52"/>
-      <c r="Y39" s="51" t="s">
+      <c r="N39" s="70"/>
+      <c r="O39" s="70"/>
+      <c r="P39" s="70"/>
+      <c r="Q39" s="70"/>
+      <c r="R39" s="70"/>
+      <c r="S39" s="70"/>
+      <c r="T39" s="70"/>
+      <c r="U39" s="70"/>
+      <c r="V39" s="70"/>
+      <c r="W39" s="70"/>
+      <c r="X39" s="73"/>
+      <c r="Y39" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="Z39" s="49"/>
-      <c r="AA39" s="49"/>
-      <c r="AB39" s="49"/>
-      <c r="AC39" s="49"/>
-      <c r="AD39" s="49"/>
-      <c r="AE39" s="49"/>
-      <c r="AF39" s="49"/>
-      <c r="AG39" s="49"/>
-      <c r="AH39" s="49"/>
-      <c r="AI39" s="49"/>
-      <c r="AJ39" s="52"/>
-    </row>
-    <row r="40" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="53" t="s">
+      <c r="Z39" s="70"/>
+      <c r="AA39" s="70"/>
+      <c r="AB39" s="70"/>
+      <c r="AC39" s="70"/>
+      <c r="AD39" s="70"/>
+      <c r="AE39" s="70"/>
+      <c r="AF39" s="70"/>
+      <c r="AG39" s="70"/>
+      <c r="AH39" s="70"/>
+      <c r="AI39" s="70"/>
+      <c r="AJ39" s="73"/>
+    </row>
+    <row r="40" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="54"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="54" t="s">
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="J40" s="54"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="55"/>
-      <c r="M40" s="56" t="s">
+      <c r="J40" s="65"/>
+      <c r="K40" s="65"/>
+      <c r="L40" s="67"/>
+      <c r="M40" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="N40" s="54"/>
-      <c r="O40" s="54"/>
-      <c r="P40" s="54"/>
-      <c r="Q40" s="54"/>
-      <c r="R40" s="54"/>
-      <c r="S40" s="54"/>
-      <c r="T40" s="54"/>
-      <c r="U40" s="54" t="s">
+      <c r="N40" s="65"/>
+      <c r="O40" s="65"/>
+      <c r="P40" s="65"/>
+      <c r="Q40" s="65"/>
+      <c r="R40" s="65"/>
+      <c r="S40" s="65"/>
+      <c r="T40" s="65"/>
+      <c r="U40" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="V40" s="54"/>
-      <c r="W40" s="54"/>
-      <c r="X40" s="57"/>
-      <c r="Y40" s="56" t="s">
+      <c r="V40" s="65"/>
+      <c r="W40" s="65"/>
+      <c r="X40" s="66"/>
+      <c r="Y40" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="Z40" s="54"/>
-      <c r="AA40" s="54"/>
-      <c r="AB40" s="54"/>
-      <c r="AC40" s="54"/>
-      <c r="AD40" s="54"/>
-      <c r="AE40" s="54"/>
-      <c r="AF40" s="54"/>
-      <c r="AG40" s="54" t="s">
+      <c r="Z40" s="65"/>
+      <c r="AA40" s="65"/>
+      <c r="AB40" s="65"/>
+      <c r="AC40" s="65"/>
+      <c r="AD40" s="65"/>
+      <c r="AE40" s="65"/>
+      <c r="AF40" s="65"/>
+      <c r="AG40" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="AH40" s="54"/>
-      <c r="AI40" s="54"/>
-      <c r="AJ40" s="57"/>
-    </row>
-    <row r="41" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH40" s="65"/>
+      <c r="AI40" s="65"/>
+      <c r="AJ40" s="66"/>
+    </row>
+    <row r="41" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="23"/>
       <c r="D41" s="23"/>
-      <c r="E41" s="54" t="s">
+      <c r="E41" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="54"/>
-      <c r="I41" s="54" t="s">
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="65"/>
+      <c r="I41" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="54"/>
-      <c r="K41" s="54"/>
-      <c r="L41" s="55"/>
+      <c r="J41" s="65"/>
+      <c r="K41" s="65"/>
+      <c r="L41" s="67"/>
       <c r="M41" s="24" t="s">
         <v>22</v>
       </c>
       <c r="N41" s="23"/>
       <c r="O41" s="23"/>
       <c r="P41" s="23"/>
-      <c r="Q41" s="54" t="s">
+      <c r="Q41" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="R41" s="54"/>
-      <c r="S41" s="54"/>
-      <c r="T41" s="54"/>
-      <c r="U41" s="54" t="s">
+      <c r="R41" s="65"/>
+      <c r="S41" s="65"/>
+      <c r="T41" s="65"/>
+      <c r="U41" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="V41" s="54"/>
-      <c r="W41" s="54"/>
-      <c r="X41" s="57"/>
+      <c r="V41" s="65"/>
+      <c r="W41" s="65"/>
+      <c r="X41" s="66"/>
       <c r="Y41" s="24" t="s">
         <v>22</v>
       </c>
       <c r="Z41" s="23"/>
       <c r="AA41" s="23"/>
       <c r="AB41" s="23"/>
-      <c r="AC41" s="54" t="s">
+      <c r="AC41" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AD41" s="54"/>
-      <c r="AE41" s="54"/>
-      <c r="AF41" s="54"/>
-      <c r="AG41" s="54" t="s">
+      <c r="AD41" s="65"/>
+      <c r="AE41" s="65"/>
+      <c r="AF41" s="65"/>
+      <c r="AG41" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="AH41" s="54"/>
-      <c r="AI41" s="54"/>
-      <c r="AJ41" s="57"/>
-    </row>
-    <row r="42" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AH41" s="65"/>
+      <c r="AI41" s="65"/>
+      <c r="AJ41" s="66"/>
+    </row>
+    <row r="42" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="28"/>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
@@ -3541,39 +3574,39 @@
       <c r="AI42" s="84"/>
       <c r="AJ42" s="86"/>
     </row>
-    <row r="43" spans="1:36" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="75" t="s">
+    <row r="43" spans="1:36" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="76"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="77"/>
-      <c r="J43" s="75" t="s">
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="K43" s="76"/>
-      <c r="L43" s="78"/>
-      <c r="M43" s="75" t="s">
+      <c r="K43" s="47"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="N43" s="76"/>
-      <c r="O43" s="76"/>
-      <c r="P43" s="76"/>
-      <c r="Q43" s="76"/>
-      <c r="R43" s="76"/>
-      <c r="S43" s="76"/>
-      <c r="T43" s="76"/>
-      <c r="U43" s="77"/>
-      <c r="V43" s="75" t="s">
+      <c r="N43" s="47"/>
+      <c r="O43" s="47"/>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="47"/>
+      <c r="S43" s="47"/>
+      <c r="T43" s="47"/>
+      <c r="U43" s="48"/>
+      <c r="V43" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="W43" s="76"/>
-      <c r="X43" s="78"/>
+      <c r="W43" s="47"/>
+      <c r="X43" s="49"/>
       <c r="Y43" s="80" t="s">
         <v>16</v>
       </c>
@@ -3591,7 +3624,7 @@
       <c r="AI43" s="81"/>
       <c r="AJ43" s="82"/>
     </row>
-    <row r="44" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="s">
         <v>50</v>
       </c>
@@ -3603,11 +3636,11 @@
       <c r="G44" s="36"/>
       <c r="H44" s="36"/>
       <c r="I44" s="39"/>
-      <c r="J44" s="71" t="s">
+      <c r="J44" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="K44" s="72"/>
-      <c r="L44" s="73"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="54"/>
       <c r="M44" s="40" t="s">
         <v>47</v>
       </c>
@@ -3619,11 +3652,11 @@
       <c r="S44" s="36"/>
       <c r="T44" s="36"/>
       <c r="U44" s="39"/>
-      <c r="V44" s="71" t="s">
+      <c r="V44" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="W44" s="72"/>
-      <c r="X44" s="73"/>
+      <c r="W44" s="43"/>
+      <c r="X44" s="54"/>
       <c r="Y44" s="40" t="s">
         <v>63</v>
       </c>
@@ -3635,63 +3668,63 @@
       <c r="AE44" s="36"/>
       <c r="AF44" s="36"/>
       <c r="AG44" s="39"/>
-      <c r="AH44" s="71" t="s">
+      <c r="AH44" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="AI44" s="72"/>
-      <c r="AJ44" s="74"/>
-    </row>
-    <row r="45" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="75" t="s">
+      <c r="AI44" s="43"/>
+      <c r="AJ44" s="55"/>
+    </row>
+    <row r="45" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="76"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="76"/>
-      <c r="F45" s="76"/>
-      <c r="G45" s="76"/>
-      <c r="H45" s="76"/>
-      <c r="I45" s="77"/>
-      <c r="J45" s="75" t="s">
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="K45" s="76"/>
-      <c r="L45" s="78"/>
-      <c r="M45" s="75" t="s">
+      <c r="K45" s="47"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="N45" s="76"/>
-      <c r="O45" s="76"/>
-      <c r="P45" s="76"/>
-      <c r="Q45" s="76"/>
-      <c r="R45" s="76"/>
-      <c r="S45" s="76"/>
-      <c r="T45" s="76"/>
-      <c r="U45" s="77"/>
-      <c r="V45" s="75" t="s">
+      <c r="N45" s="47"/>
+      <c r="O45" s="47"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="47"/>
+      <c r="R45" s="47"/>
+      <c r="S45" s="47"/>
+      <c r="T45" s="47"/>
+      <c r="U45" s="48"/>
+      <c r="V45" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="W45" s="76"/>
-      <c r="X45" s="78"/>
-      <c r="Y45" s="79" t="s">
+      <c r="W45" s="47"/>
+      <c r="X45" s="49"/>
+      <c r="Y45" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="Z45" s="76"/>
-      <c r="AA45" s="76"/>
-      <c r="AB45" s="76"/>
-      <c r="AC45" s="76"/>
-      <c r="AD45" s="76"/>
-      <c r="AE45" s="76"/>
-      <c r="AF45" s="76"/>
-      <c r="AG45" s="77"/>
-      <c r="AH45" s="75" t="s">
+      <c r="Z45" s="47"/>
+      <c r="AA45" s="47"/>
+      <c r="AB45" s="47"/>
+      <c r="AC45" s="47"/>
+      <c r="AD45" s="47"/>
+      <c r="AE45" s="47"/>
+      <c r="AF45" s="47"/>
+      <c r="AG45" s="48"/>
+      <c r="AH45" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="AI45" s="76"/>
-      <c r="AJ45" s="77"/>
-    </row>
-    <row r="46" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AI45" s="47"/>
+      <c r="AJ45" s="48"/>
+    </row>
+    <row r="46" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="40" t="s">
         <v>54</v>
       </c>
@@ -3703,11 +3736,11 @@
       <c r="G46" s="36"/>
       <c r="H46" s="36"/>
       <c r="I46" s="39"/>
-      <c r="J46" s="71" t="s">
+      <c r="J46" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="K46" s="72"/>
-      <c r="L46" s="73"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="54"/>
       <c r="M46" s="38" t="s">
         <v>60</v>
       </c>
@@ -3719,11 +3752,11 @@
       <c r="S46" s="36"/>
       <c r="T46" s="36"/>
       <c r="U46" s="39"/>
-      <c r="V46" s="71" t="s">
+      <c r="V46" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="W46" s="72"/>
-      <c r="X46" s="73"/>
+      <c r="W46" s="43"/>
+      <c r="X46" s="54"/>
       <c r="Y46" s="38" t="s">
         <v>59</v>
       </c>
@@ -3735,13 +3768,13 @@
       <c r="AE46" s="36"/>
       <c r="AF46" s="36"/>
       <c r="AG46" s="39"/>
-      <c r="AH46" s="71" t="s">
+      <c r="AH46" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="AI46" s="72"/>
-      <c r="AJ46" s="74"/>
-    </row>
-    <row r="47" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AI46" s="43"/>
+      <c r="AJ46" s="55"/>
+    </row>
+    <row r="47" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="40"/>
       <c r="B47" s="36"/>
       <c r="C47" s="36"/>
@@ -3751,9 +3784,9 @@
       <c r="G47" s="36"/>
       <c r="H47" s="36"/>
       <c r="I47" s="39"/>
-      <c r="J47" s="71"/>
-      <c r="K47" s="72"/>
-      <c r="L47" s="73"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="54"/>
       <c r="M47" s="40"/>
       <c r="N47" s="36"/>
       <c r="O47" s="36"/>
@@ -3763,9 +3796,9 @@
       <c r="S47" s="36"/>
       <c r="T47" s="36"/>
       <c r="U47" s="39"/>
-      <c r="V47" s="71"/>
-      <c r="W47" s="72"/>
-      <c r="X47" s="73"/>
+      <c r="V47" s="53"/>
+      <c r="W47" s="43"/>
+      <c r="X47" s="54"/>
       <c r="Y47" s="38"/>
       <c r="Z47" s="36"/>
       <c r="AA47" s="36"/>
@@ -3775,11 +3808,11 @@
       <c r="AE47" s="36"/>
       <c r="AF47" s="36"/>
       <c r="AG47" s="39"/>
-      <c r="AH47" s="71"/>
-      <c r="AI47" s="72"/>
-      <c r="AJ47" s="74"/>
-    </row>
-    <row r="48" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH47" s="53"/>
+      <c r="AI47" s="43"/>
+      <c r="AJ47" s="55"/>
+    </row>
+    <row r="48" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="40"/>
       <c r="B48" s="36"/>
       <c r="C48" s="36"/>
@@ -3789,9 +3822,9 @@
       <c r="G48" s="36"/>
       <c r="H48" s="36"/>
       <c r="I48" s="39"/>
-      <c r="J48" s="71"/>
-      <c r="K48" s="72"/>
-      <c r="L48" s="73"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="54"/>
       <c r="M48" s="40"/>
       <c r="N48" s="36"/>
       <c r="O48" s="36"/>
@@ -3801,9 +3834,9 @@
       <c r="S48" s="36"/>
       <c r="T48" s="36"/>
       <c r="U48" s="39"/>
-      <c r="V48" s="71"/>
-      <c r="W48" s="72"/>
-      <c r="X48" s="73"/>
+      <c r="V48" s="53"/>
+      <c r="W48" s="43"/>
+      <c r="X48" s="54"/>
       <c r="Y48" s="38"/>
       <c r="Z48" s="36"/>
       <c r="AA48" s="36"/>
@@ -3813,11 +3846,11 @@
       <c r="AE48" s="36"/>
       <c r="AF48" s="36"/>
       <c r="AG48" s="39"/>
-      <c r="AH48" s="71"/>
-      <c r="AI48" s="72"/>
-      <c r="AJ48" s="74"/>
-    </row>
-    <row r="49" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH48" s="53"/>
+      <c r="AI48" s="43"/>
+      <c r="AJ48" s="55"/>
+    </row>
+    <row r="49" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
       <c r="B49" s="36"/>
       <c r="C49" s="36"/>
@@ -3827,9 +3860,9 @@
       <c r="G49" s="36"/>
       <c r="H49" s="36"/>
       <c r="I49" s="39"/>
-      <c r="J49" s="71"/>
-      <c r="K49" s="72"/>
-      <c r="L49" s="73"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="54"/>
       <c r="M49" s="40"/>
       <c r="N49" s="36"/>
       <c r="O49" s="36"/>
@@ -3839,9 +3872,9 @@
       <c r="S49" s="36"/>
       <c r="T49" s="36"/>
       <c r="U49" s="39"/>
-      <c r="V49" s="71"/>
-      <c r="W49" s="72"/>
-      <c r="X49" s="73"/>
+      <c r="V49" s="53"/>
+      <c r="W49" s="43"/>
+      <c r="X49" s="54"/>
       <c r="Y49" s="38"/>
       <c r="Z49" s="36"/>
       <c r="AA49" s="36"/>
@@ -3851,329 +3884,329 @@
       <c r="AE49" s="36"/>
       <c r="AF49" s="36"/>
       <c r="AG49" s="39"/>
-      <c r="AH49" s="71"/>
-      <c r="AI49" s="72"/>
-      <c r="AJ49" s="74"/>
-    </row>
-    <row r="50" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="61" t="s">
+      <c r="AH49" s="53"/>
+      <c r="AI49" s="43"/>
+      <c r="AJ49" s="55"/>
+    </row>
+    <row r="50" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="62"/>
-      <c r="C50" s="62"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="62"/>
-      <c r="F50" s="62"/>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
-      <c r="L50" s="63"/>
-      <c r="M50" s="64" t="s">
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="N50" s="62"/>
-      <c r="O50" s="62"/>
-      <c r="P50" s="62"/>
-      <c r="Q50" s="62"/>
-      <c r="R50" s="62"/>
-      <c r="S50" s="62"/>
-      <c r="T50" s="62"/>
-      <c r="U50" s="62"/>
-      <c r="V50" s="62"/>
-      <c r="W50" s="62"/>
-      <c r="X50" s="65"/>
-      <c r="Y50" s="64" t="s">
+      <c r="N50" s="57"/>
+      <c r="O50" s="57"/>
+      <c r="P50" s="57"/>
+      <c r="Q50" s="57"/>
+      <c r="R50" s="57"/>
+      <c r="S50" s="57"/>
+      <c r="T50" s="57"/>
+      <c r="U50" s="57"/>
+      <c r="V50" s="57"/>
+      <c r="W50" s="57"/>
+      <c r="X50" s="60"/>
+      <c r="Y50" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="Z50" s="62"/>
-      <c r="AA50" s="62"/>
-      <c r="AB50" s="62"/>
-      <c r="AC50" s="62"/>
-      <c r="AD50" s="62"/>
-      <c r="AE50" s="62"/>
-      <c r="AF50" s="62"/>
-      <c r="AG50" s="62"/>
-      <c r="AH50" s="62"/>
-      <c r="AI50" s="62"/>
-      <c r="AJ50" s="65"/>
-    </row>
-    <row r="51" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="66" t="s">
+      <c r="Z50" s="57"/>
+      <c r="AA50" s="57"/>
+      <c r="AB50" s="57"/>
+      <c r="AC50" s="57"/>
+      <c r="AD50" s="57"/>
+      <c r="AE50" s="57"/>
+      <c r="AF50" s="57"/>
+      <c r="AG50" s="57"/>
+      <c r="AH50" s="57"/>
+      <c r="AI50" s="57"/>
+      <c r="AJ50" s="60"/>
+    </row>
+    <row r="51" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="67"/>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
-      <c r="E51" s="67"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
       <c r="F51" s="41">
         <v>6</v>
       </c>
       <c r="G51" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H51" s="67" t="s">
+      <c r="H51" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="I51" s="67"/>
+      <c r="I51" s="62"/>
       <c r="J51" s="41">
         <v>40</v>
       </c>
-      <c r="K51" s="68" t="s">
+      <c r="K51" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="L51" s="69"/>
-      <c r="M51" s="66" t="s">
+      <c r="L51" s="64"/>
+      <c r="M51" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="N51" s="67"/>
-      <c r="O51" s="67"/>
-      <c r="P51" s="67"/>
-      <c r="Q51" s="67"/>
+      <c r="N51" s="62"/>
+      <c r="O51" s="62"/>
+      <c r="P51" s="62"/>
+      <c r="Q51" s="62"/>
       <c r="R51" s="41">
         <v>6</v>
       </c>
       <c r="S51" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="T51" s="67" t="s">
+      <c r="T51" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="U51" s="67"/>
+      <c r="U51" s="62"/>
       <c r="V51" s="41">
         <v>40</v>
       </c>
-      <c r="W51" s="68" t="s">
+      <c r="W51" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="X51" s="69"/>
-      <c r="Y51" s="66" t="s">
+      <c r="X51" s="64"/>
+      <c r="Y51" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Z51" s="67"/>
-      <c r="AA51" s="67"/>
-      <c r="AB51" s="67"/>
-      <c r="AC51" s="67"/>
+      <c r="Z51" s="62"/>
+      <c r="AA51" s="62"/>
+      <c r="AB51" s="62"/>
+      <c r="AC51" s="62"/>
       <c r="AD51" s="41">
         <v>6</v>
       </c>
       <c r="AE51" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="AF51" s="67" t="s">
+      <c r="AF51" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="AG51" s="67"/>
+      <c r="AG51" s="62"/>
       <c r="AH51" s="41">
         <v>40</v>
       </c>
-      <c r="AI51" s="68" t="s">
+      <c r="AI51" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AJ51" s="70"/>
-    </row>
-    <row r="52" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="48" t="s">
+      <c r="AJ51" s="68"/>
+    </row>
+    <row r="52" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B52" s="49"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="49"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="49"/>
-      <c r="H52" s="49"/>
-      <c r="I52" s="49"/>
-      <c r="J52" s="49"/>
-      <c r="K52" s="49"/>
-      <c r="L52" s="50"/>
-      <c r="M52" s="51" t="s">
+      <c r="B52" s="70"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="70"/>
+      <c r="E52" s="70"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="70"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="70"/>
+      <c r="J52" s="70"/>
+      <c r="K52" s="70"/>
+      <c r="L52" s="71"/>
+      <c r="M52" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="N52" s="49"/>
-      <c r="O52" s="49"/>
-      <c r="P52" s="49"/>
-      <c r="Q52" s="49"/>
-      <c r="R52" s="49"/>
-      <c r="S52" s="49"/>
-      <c r="T52" s="49"/>
-      <c r="U52" s="49"/>
-      <c r="V52" s="49"/>
-      <c r="W52" s="49"/>
-      <c r="X52" s="52"/>
-      <c r="Y52" s="51" t="s">
+      <c r="N52" s="70"/>
+      <c r="O52" s="70"/>
+      <c r="P52" s="70"/>
+      <c r="Q52" s="70"/>
+      <c r="R52" s="70"/>
+      <c r="S52" s="70"/>
+      <c r="T52" s="70"/>
+      <c r="U52" s="70"/>
+      <c r="V52" s="70"/>
+      <c r="W52" s="70"/>
+      <c r="X52" s="73"/>
+      <c r="Y52" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="Z52" s="49"/>
-      <c r="AA52" s="49"/>
-      <c r="AB52" s="49"/>
-      <c r="AC52" s="49"/>
-      <c r="AD52" s="49"/>
-      <c r="AE52" s="49"/>
-      <c r="AF52" s="49"/>
-      <c r="AG52" s="49"/>
-      <c r="AH52" s="49"/>
-      <c r="AI52" s="49"/>
-      <c r="AJ52" s="52"/>
-    </row>
-    <row r="53" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="53" t="s">
+      <c r="Z52" s="70"/>
+      <c r="AA52" s="70"/>
+      <c r="AB52" s="70"/>
+      <c r="AC52" s="70"/>
+      <c r="AD52" s="70"/>
+      <c r="AE52" s="70"/>
+      <c r="AF52" s="70"/>
+      <c r="AG52" s="70"/>
+      <c r="AH52" s="70"/>
+      <c r="AI52" s="70"/>
+      <c r="AJ52" s="73"/>
+    </row>
+    <row r="53" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="54"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="54"/>
-      <c r="I53" s="54" t="s">
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="65"/>
+      <c r="H53" s="65"/>
+      <c r="I53" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="J53" s="54"/>
-      <c r="K53" s="54"/>
-      <c r="L53" s="55"/>
-      <c r="M53" s="56" t="s">
+      <c r="J53" s="65"/>
+      <c r="K53" s="65"/>
+      <c r="L53" s="67"/>
+      <c r="M53" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="N53" s="54"/>
-      <c r="O53" s="54"/>
-      <c r="P53" s="54"/>
-      <c r="Q53" s="54"/>
-      <c r="R53" s="54"/>
-      <c r="S53" s="54"/>
-      <c r="T53" s="54"/>
-      <c r="U53" s="54" t="s">
+      <c r="N53" s="65"/>
+      <c r="O53" s="65"/>
+      <c r="P53" s="65"/>
+      <c r="Q53" s="65"/>
+      <c r="R53" s="65"/>
+      <c r="S53" s="65"/>
+      <c r="T53" s="65"/>
+      <c r="U53" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="V53" s="54"/>
-      <c r="W53" s="54"/>
-      <c r="X53" s="57"/>
-      <c r="Y53" s="56" t="s">
+      <c r="V53" s="65"/>
+      <c r="W53" s="65"/>
+      <c r="X53" s="66"/>
+      <c r="Y53" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="Z53" s="54"/>
-      <c r="AA53" s="54"/>
-      <c r="AB53" s="54"/>
-      <c r="AC53" s="54"/>
-      <c r="AD53" s="54"/>
-      <c r="AE53" s="54"/>
-      <c r="AF53" s="54"/>
-      <c r="AG53" s="54" t="s">
+      <c r="Z53" s="65"/>
+      <c r="AA53" s="65"/>
+      <c r="AB53" s="65"/>
+      <c r="AC53" s="65"/>
+      <c r="AD53" s="65"/>
+      <c r="AE53" s="65"/>
+      <c r="AF53" s="65"/>
+      <c r="AG53" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="AH53" s="54"/>
-      <c r="AI53" s="54"/>
-      <c r="AJ53" s="57"/>
-    </row>
-    <row r="54" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH53" s="65"/>
+      <c r="AI53" s="65"/>
+      <c r="AJ53" s="66"/>
+    </row>
+    <row r="54" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B54" s="23"/>
       <c r="C54" s="23"/>
       <c r="D54" s="23"/>
-      <c r="E54" s="54" t="s">
+      <c r="E54" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="F54" s="54"/>
-      <c r="G54" s="54"/>
-      <c r="H54" s="54"/>
-      <c r="I54" s="54" t="s">
+      <c r="F54" s="65"/>
+      <c r="G54" s="65"/>
+      <c r="H54" s="65"/>
+      <c r="I54" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="J54" s="54"/>
-      <c r="K54" s="54"/>
-      <c r="L54" s="55"/>
+      <c r="J54" s="65"/>
+      <c r="K54" s="65"/>
+      <c r="L54" s="67"/>
       <c r="M54" s="24" t="s">
         <v>22</v>
       </c>
       <c r="N54" s="23"/>
       <c r="O54" s="23"/>
       <c r="P54" s="23"/>
-      <c r="Q54" s="54" t="s">
+      <c r="Q54" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="R54" s="54"/>
-      <c r="S54" s="54"/>
-      <c r="T54" s="54"/>
-      <c r="U54" s="54" t="s">
+      <c r="R54" s="65"/>
+      <c r="S54" s="65"/>
+      <c r="T54" s="65"/>
+      <c r="U54" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="V54" s="54"/>
-      <c r="W54" s="54"/>
-      <c r="X54" s="57"/>
+      <c r="V54" s="65"/>
+      <c r="W54" s="65"/>
+      <c r="X54" s="66"/>
       <c r="Y54" s="24" t="s">
         <v>22</v>
       </c>
       <c r="Z54" s="23"/>
       <c r="AA54" s="23"/>
       <c r="AB54" s="23"/>
-      <c r="AC54" s="54" t="s">
+      <c r="AC54" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AD54" s="54"/>
-      <c r="AE54" s="54"/>
-      <c r="AF54" s="54"/>
-      <c r="AG54" s="54" t="s">
+      <c r="AD54" s="65"/>
+      <c r="AE54" s="65"/>
+      <c r="AF54" s="65"/>
+      <c r="AG54" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="AH54" s="54"/>
-      <c r="AI54" s="54"/>
-      <c r="AJ54" s="57"/>
-    </row>
-    <row r="55" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH54" s="65"/>
+      <c r="AI54" s="65"/>
+      <c r="AJ54" s="66"/>
+    </row>
+    <row r="55" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="29"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
-      <c r="E55" s="58" t="s">
+      <c r="E55" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="58" t="s">
+      <c r="F55" s="87"/>
+      <c r="G55" s="87"/>
+      <c r="H55" s="87"/>
+      <c r="I55" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="J55" s="58"/>
-      <c r="K55" s="58"/>
-      <c r="L55" s="59"/>
+      <c r="J55" s="87"/>
+      <c r="K55" s="87"/>
+      <c r="L55" s="88"/>
       <c r="M55" s="31"/>
       <c r="N55" s="30"/>
       <c r="O55" s="30"/>
       <c r="P55" s="30"/>
-      <c r="Q55" s="58" t="s">
+      <c r="Q55" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="R55" s="58"/>
-      <c r="S55" s="58"/>
-      <c r="T55" s="58"/>
-      <c r="U55" s="58" t="s">
+      <c r="R55" s="87"/>
+      <c r="S55" s="87"/>
+      <c r="T55" s="87"/>
+      <c r="U55" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="V55" s="58"/>
-      <c r="W55" s="58"/>
-      <c r="X55" s="60"/>
+      <c r="V55" s="87"/>
+      <c r="W55" s="87"/>
+      <c r="X55" s="89"/>
       <c r="Y55" s="31"/>
       <c r="Z55" s="30"/>
       <c r="AA55" s="30"/>
       <c r="AB55" s="30"/>
-      <c r="AC55" s="58" t="s">
+      <c r="AC55" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="AD55" s="58"/>
-      <c r="AE55" s="58"/>
-      <c r="AF55" s="58"/>
-      <c r="AG55" s="58" t="s">
+      <c r="AD55" s="87"/>
+      <c r="AE55" s="87"/>
+      <c r="AF55" s="87"/>
+      <c r="AG55" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="AH55" s="58"/>
-      <c r="AI55" s="58"/>
-      <c r="AJ55" s="60"/>
-    </row>
-    <row r="56" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH55" s="87"/>
+      <c r="AI55" s="87"/>
+      <c r="AJ55" s="89"/>
+    </row>
+    <row r="56" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
         <v>24</v>
       </c>
@@ -4181,280 +4214,125 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z57" s="45" t="s">
+      <c r="Z57" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="AA57" s="45"/>
-      <c r="AB57" s="45"/>
-      <c r="AC57" s="45"/>
-      <c r="AD57" s="45"/>
-      <c r="AE57" s="45"/>
-      <c r="AF57" s="45"/>
-      <c r="AG57" s="45"/>
-      <c r="AH57" s="46">
+      <c r="AA57" s="92"/>
+      <c r="AB57" s="92"/>
+      <c r="AC57" s="92"/>
+      <c r="AD57" s="92"/>
+      <c r="AE57" s="92"/>
+      <c r="AF57" s="92"/>
+      <c r="AG57" s="92"/>
+      <c r="AH57" s="93">
         <v>35</v>
       </c>
-      <c r="AI57" s="46"/>
-      <c r="AJ57" s="46"/>
-    </row>
-    <row r="58" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AI57" s="93"/>
+      <c r="AJ57" s="93"/>
+    </row>
+    <row r="58" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z58" s="45" t="s">
+      <c r="Z58" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="AA58" s="45"/>
-      <c r="AB58" s="45"/>
-      <c r="AC58" s="45"/>
-      <c r="AD58" s="45"/>
-      <c r="AE58" s="45"/>
-      <c r="AF58" s="45"/>
-      <c r="AG58" s="45"/>
-      <c r="AH58" s="46">
+      <c r="AA58" s="92"/>
+      <c r="AB58" s="92"/>
+      <c r="AC58" s="92"/>
+      <c r="AD58" s="92"/>
+      <c r="AE58" s="92"/>
+      <c r="AF58" s="92"/>
+      <c r="AG58" s="92"/>
+      <c r="AH58" s="93">
         <v>0</v>
       </c>
-      <c r="AI58" s="46"/>
-      <c r="AJ58" s="46"/>
-    </row>
-    <row r="59" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AI58" s="93"/>
+      <c r="AJ58" s="93"/>
+    </row>
+    <row r="59" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Z59" s="47" t="s">
+      <c r="Z59" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="AA59" s="47"/>
-      <c r="AB59" s="47"/>
-      <c r="AC59" s="47"/>
-      <c r="AD59" s="47"/>
-      <c r="AE59" s="47"/>
-      <c r="AF59" s="47"/>
-      <c r="AG59" s="47"/>
-      <c r="AH59" s="46">
+      <c r="AA59" s="94"/>
+      <c r="AB59" s="94"/>
+      <c r="AC59" s="94"/>
+      <c r="AD59" s="94"/>
+      <c r="AE59" s="94"/>
+      <c r="AF59" s="94"/>
+      <c r="AG59" s="94"/>
+      <c r="AH59" s="93">
         <v>35</v>
       </c>
-      <c r="AI59" s="46"/>
-      <c r="AJ59" s="46"/>
-    </row>
-    <row r="60" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="Z60" s="43" t="s">
+      <c r="AI59" s="93"/>
+      <c r="AJ59" s="93"/>
+    </row>
+    <row r="60" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z60" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="AA60" s="43"/>
-      <c r="AB60" s="43"/>
-      <c r="AC60" s="43"/>
-      <c r="AD60" s="43"/>
-      <c r="AE60" s="43"/>
-      <c r="AF60" s="43"/>
-      <c r="AG60" s="43"/>
-      <c r="AH60" s="43"/>
-      <c r="AI60" s="43"/>
-      <c r="AJ60" s="43"/>
-    </row>
-    <row r="61" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AA60" s="90"/>
+      <c r="AB60" s="90"/>
+      <c r="AC60" s="90"/>
+      <c r="AD60" s="90"/>
+      <c r="AE60" s="90"/>
+      <c r="AF60" s="90"/>
+      <c r="AG60" s="90"/>
+      <c r="AH60" s="90"/>
+      <c r="AI60" s="90"/>
+      <c r="AJ60" s="90"/>
+    </row>
+    <row r="61" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="Z61" s="44" t="s">
+      <c r="Z61" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="AA61" s="44"/>
-      <c r="AB61" s="44"/>
-      <c r="AC61" s="44"/>
-      <c r="AD61" s="44"/>
-      <c r="AE61" s="44"/>
-      <c r="AF61" s="44"/>
-      <c r="AG61" s="44"/>
-      <c r="AH61" s="44"/>
-      <c r="AI61" s="44"/>
-      <c r="AJ61" s="44"/>
-    </row>
-    <row r="62" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="Z62" s="44" t="s">
+      <c r="AA61" s="91"/>
+      <c r="AB61" s="91"/>
+      <c r="AC61" s="91"/>
+      <c r="AD61" s="91"/>
+      <c r="AE61" s="91"/>
+      <c r="AF61" s="91"/>
+      <c r="AG61" s="91"/>
+      <c r="AH61" s="91"/>
+      <c r="AI61" s="91"/>
+      <c r="AJ61" s="91"/>
+    </row>
+    <row r="62" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z62" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="AA62" s="44"/>
-      <c r="AB62" s="44"/>
-      <c r="AC62" s="44"/>
-      <c r="AD62" s="44"/>
-      <c r="AE62" s="44"/>
-      <c r="AF62" s="44"/>
-      <c r="AG62" s="44"/>
-      <c r="AH62" s="44"/>
-      <c r="AI62" s="44"/>
-      <c r="AJ62" s="44"/>
+      <c r="AA62" s="91"/>
+      <c r="AB62" s="91"/>
+      <c r="AC62" s="91"/>
+      <c r="AD62" s="91"/>
+      <c r="AE62" s="91"/>
+      <c r="AF62" s="91"/>
+      <c r="AG62" s="91"/>
+      <c r="AH62" s="91"/>
+      <c r="AI62" s="91"/>
+      <c r="AJ62" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="194">
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="A6:AH6"/>
-    <mergeCell ref="A7:AH7"/>
-    <mergeCell ref="A16:AJ16"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M17:U17"/>
-    <mergeCell ref="V17:X17"/>
-    <mergeCell ref="Y17:AG17"/>
-    <mergeCell ref="AH17:AJ17"/>
-    <mergeCell ref="Z3:AC3"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="V18:X18"/>
-    <mergeCell ref="AH18:AJ18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M19:U19"/>
-    <mergeCell ref="V19:X19"/>
-    <mergeCell ref="Y19:AG19"/>
-    <mergeCell ref="AH19:AJ19"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="V22:X22"/>
-    <mergeCell ref="AH22:AJ22"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="AH23:AJ23"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="V20:X20"/>
-    <mergeCell ref="AH20:AJ20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="V21:X21"/>
-    <mergeCell ref="AH21:AJ21"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="M24:X24"/>
-    <mergeCell ref="Y24:AJ24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:Q25"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y25:AC25"/>
-    <mergeCell ref="AG27:AJ27"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="Q28:T28"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="AC28:AF28"/>
-    <mergeCell ref="AG28:AJ28"/>
-    <mergeCell ref="AF25:AG25"/>
-    <mergeCell ref="AI25:AJ25"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="M26:X26"/>
-    <mergeCell ref="Y26:AJ26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="M27:T27"/>
-    <mergeCell ref="U27:X27"/>
-    <mergeCell ref="Y27:AF27"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="M30:U30"/>
-    <mergeCell ref="V30:X30"/>
-    <mergeCell ref="Y30:AG30"/>
-    <mergeCell ref="AH30:AJ30"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="Q29:T29"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="AC29:AF29"/>
-    <mergeCell ref="AG29:AJ29"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="V31:X31"/>
-    <mergeCell ref="AH31:AJ31"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="M32:U32"/>
-    <mergeCell ref="V32:X32"/>
-    <mergeCell ref="Y32:AG32"/>
-    <mergeCell ref="AH32:AJ32"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="V35:X35"/>
-    <mergeCell ref="AH35:AJ35"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="V36:X36"/>
-    <mergeCell ref="AH36:AJ36"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="V33:X33"/>
-    <mergeCell ref="AH33:AJ33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="V34:X34"/>
-    <mergeCell ref="AH34:AJ34"/>
-    <mergeCell ref="A37:L37"/>
-    <mergeCell ref="M37:X37"/>
-    <mergeCell ref="Y37:AJ37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="M38:Q38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="W38:X38"/>
-    <mergeCell ref="Y38:AC38"/>
-    <mergeCell ref="AG40:AJ40"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="Q41:T41"/>
-    <mergeCell ref="U41:X41"/>
-    <mergeCell ref="AC41:AF41"/>
-    <mergeCell ref="AG41:AJ41"/>
-    <mergeCell ref="AF38:AG38"/>
-    <mergeCell ref="AI38:AJ38"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="M39:X39"/>
-    <mergeCell ref="Y39:AJ39"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="M40:T40"/>
-    <mergeCell ref="U40:X40"/>
-    <mergeCell ref="Y40:AF40"/>
-    <mergeCell ref="A43:I43"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="M43:U43"/>
-    <mergeCell ref="V43:X43"/>
-    <mergeCell ref="Y43:AG43"/>
-    <mergeCell ref="AH43:AJ43"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="Q42:T42"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="AC42:AF42"/>
-    <mergeCell ref="AG42:AJ42"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="V44:X44"/>
-    <mergeCell ref="AH44:AJ44"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="M45:U45"/>
-    <mergeCell ref="V45:X45"/>
-    <mergeCell ref="Y45:AG45"/>
-    <mergeCell ref="AH45:AJ45"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="V48:X48"/>
-    <mergeCell ref="AH48:AJ48"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="V49:X49"/>
-    <mergeCell ref="AH49:AJ49"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="V46:X46"/>
-    <mergeCell ref="AH46:AJ46"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="V47:X47"/>
-    <mergeCell ref="AH47:AJ47"/>
-    <mergeCell ref="A50:L50"/>
-    <mergeCell ref="M50:X50"/>
-    <mergeCell ref="Y50:AJ50"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="M51:Q51"/>
-    <mergeCell ref="T51:U51"/>
-    <mergeCell ref="W51:X51"/>
-    <mergeCell ref="Y51:AC51"/>
-    <mergeCell ref="AF51:AG51"/>
-    <mergeCell ref="AI51:AJ51"/>
+    <mergeCell ref="Z60:AJ60"/>
+    <mergeCell ref="Z61:AJ61"/>
+    <mergeCell ref="Z62:AJ62"/>
+    <mergeCell ref="Z57:AG57"/>
+    <mergeCell ref="AH57:AJ57"/>
+    <mergeCell ref="Z58:AG58"/>
+    <mergeCell ref="AH58:AJ58"/>
+    <mergeCell ref="Z59:AG59"/>
+    <mergeCell ref="AH59:AJ59"/>
     <mergeCell ref="A52:L52"/>
     <mergeCell ref="M52:X52"/>
     <mergeCell ref="Y52:AJ52"/>
@@ -4476,15 +4354,170 @@
     <mergeCell ref="U54:X54"/>
     <mergeCell ref="AC54:AF54"/>
     <mergeCell ref="AG54:AJ54"/>
-    <mergeCell ref="Z60:AJ60"/>
-    <mergeCell ref="Z61:AJ61"/>
-    <mergeCell ref="Z62:AJ62"/>
-    <mergeCell ref="Z57:AG57"/>
-    <mergeCell ref="AH57:AJ57"/>
-    <mergeCell ref="Z58:AG58"/>
-    <mergeCell ref="AH58:AJ58"/>
-    <mergeCell ref="Z59:AG59"/>
-    <mergeCell ref="AH59:AJ59"/>
+    <mergeCell ref="A50:L50"/>
+    <mergeCell ref="M50:X50"/>
+    <mergeCell ref="Y50:AJ50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="M51:Q51"/>
+    <mergeCell ref="T51:U51"/>
+    <mergeCell ref="W51:X51"/>
+    <mergeCell ref="Y51:AC51"/>
+    <mergeCell ref="AF51:AG51"/>
+    <mergeCell ref="AI51:AJ51"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="V48:X48"/>
+    <mergeCell ref="AH48:AJ48"/>
+    <mergeCell ref="J49:L49"/>
+    <mergeCell ref="V49:X49"/>
+    <mergeCell ref="AH49:AJ49"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="V46:X46"/>
+    <mergeCell ref="AH46:AJ46"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="V47:X47"/>
+    <mergeCell ref="AH47:AJ47"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="V44:X44"/>
+    <mergeCell ref="AH44:AJ44"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="M45:U45"/>
+    <mergeCell ref="V45:X45"/>
+    <mergeCell ref="Y45:AG45"/>
+    <mergeCell ref="AH45:AJ45"/>
+    <mergeCell ref="A43:I43"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="M43:U43"/>
+    <mergeCell ref="V43:X43"/>
+    <mergeCell ref="Y43:AG43"/>
+    <mergeCell ref="AH43:AJ43"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="Q42:T42"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="AC42:AF42"/>
+    <mergeCell ref="AG42:AJ42"/>
+    <mergeCell ref="AG40:AJ40"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="Q41:T41"/>
+    <mergeCell ref="U41:X41"/>
+    <mergeCell ref="AC41:AF41"/>
+    <mergeCell ref="AG41:AJ41"/>
+    <mergeCell ref="AF38:AG38"/>
+    <mergeCell ref="AI38:AJ38"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="M39:X39"/>
+    <mergeCell ref="Y39:AJ39"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="M40:T40"/>
+    <mergeCell ref="U40:X40"/>
+    <mergeCell ref="Y40:AF40"/>
+    <mergeCell ref="A37:L37"/>
+    <mergeCell ref="M37:X37"/>
+    <mergeCell ref="Y37:AJ37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="M38:Q38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="W38:X38"/>
+    <mergeCell ref="Y38:AC38"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="V35:X35"/>
+    <mergeCell ref="AH35:AJ35"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="V36:X36"/>
+    <mergeCell ref="AH36:AJ36"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="V33:X33"/>
+    <mergeCell ref="AH33:AJ33"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="V34:X34"/>
+    <mergeCell ref="AH34:AJ34"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="V31:X31"/>
+    <mergeCell ref="AH31:AJ31"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="M32:U32"/>
+    <mergeCell ref="V32:X32"/>
+    <mergeCell ref="Y32:AG32"/>
+    <mergeCell ref="AH32:AJ32"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="M30:U30"/>
+    <mergeCell ref="V30:X30"/>
+    <mergeCell ref="Y30:AG30"/>
+    <mergeCell ref="AH30:AJ30"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="Q29:T29"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="AC29:AF29"/>
+    <mergeCell ref="AG29:AJ29"/>
+    <mergeCell ref="AG27:AJ27"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="Q28:T28"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="AC28:AF28"/>
+    <mergeCell ref="AG28:AJ28"/>
+    <mergeCell ref="AF25:AG25"/>
+    <mergeCell ref="AI25:AJ25"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="M26:X26"/>
+    <mergeCell ref="Y26:AJ26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="M27:T27"/>
+    <mergeCell ref="U27:X27"/>
+    <mergeCell ref="Y27:AF27"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="M24:X24"/>
+    <mergeCell ref="Y24:AJ24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:Q25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="V22:X22"/>
+    <mergeCell ref="AH22:AJ22"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="AH23:AJ23"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="V20:X20"/>
+    <mergeCell ref="AH20:AJ20"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="V21:X21"/>
+    <mergeCell ref="AH21:AJ21"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="V18:X18"/>
+    <mergeCell ref="AH18:AJ18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M19:U19"/>
+    <mergeCell ref="V19:X19"/>
+    <mergeCell ref="Y19:AG19"/>
+    <mergeCell ref="AH19:AJ19"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="A6:AH6"/>
+    <mergeCell ref="A7:AH7"/>
+    <mergeCell ref="A16:AJ16"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M17:U17"/>
+    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="Y17:AG17"/>
+    <mergeCell ref="AH17:AJ17"/>
+    <mergeCell ref="Z3:AC3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -4553,7 +4586,7 @@
                     <xdr:col>30</xdr:col>
                     <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>176213</xdr:rowOff>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4567,7 +4600,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>30</xdr:col>
-                    <xdr:colOff>214313</xdr:colOff>
+                    <xdr:colOff>219075</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
@@ -4575,7 +4608,7 @@
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>176213</xdr:rowOff>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>